<commit_message>
Working on the final project
</commit_message>
<xml_diff>
--- a/projects/project-7-final/data/child_mortality_urban_1990_2021.xlsx
+++ b/projects/project-7-final/data/child_mortality_urban_1990_2021.xlsx
@@ -164,7 +164,7 @@
     <t xml:space="preserve">        Ярославская область</t>
   </si>
   <si>
-    <t xml:space="preserve">        Город Москва столица Российской Федерации город федерального значения</t>
+    <t xml:space="preserve">        Город Москва</t>
   </si>
   <si>
     <t xml:space="preserve">        Республика Карелия</t>
@@ -200,7 +200,7 @@
     <t xml:space="preserve">        Псковская область</t>
   </si>
   <si>
-    <t xml:space="preserve">        Город Санкт-Петербург город федерального значения</t>
+    <t xml:space="preserve">        Город Санкт-Петербург</t>
   </si>
   <si>
     <t xml:space="preserve">        Республика Адыгея (Адыгея)</t>

</xml_diff>